<commit_message>
Updated and tidied stock analysis scripts for sharing as thesis material
</commit_message>
<xml_diff>
--- a/scientific_common_crosswalk_raw.xlsx
+++ b/scientific_common_crosswalk_raw.xlsx
@@ -226,12 +226,12 @@
     <t xml:space="preserve">zapatero</t>
   </si>
   <si>
+    <t xml:space="preserve">jack</t>
+  </si>
+  <si>
     <t xml:space="preserve">bonita</t>
   </si>
   <si>
-    <t xml:space="preserve">jack</t>
-  </si>
-  <si>
     <t xml:space="preserve">trevally</t>
   </si>
   <si>
@@ -352,12 +352,12 @@
     <t xml:space="preserve">ronco blanco</t>
   </si>
   <si>
+    <t xml:space="preserve">ronco</t>
+  </si>
+  <si>
     <t xml:space="preserve">ronco de laguna</t>
   </si>
   <si>
-    <t xml:space="preserve">ronco</t>
-  </si>
-  <si>
     <t xml:space="preserve">Labridae</t>
   </si>
   <si>
@@ -394,87 +394,87 @@
     <t xml:space="preserve">curruncha ojuda</t>
   </si>
   <si>
+    <t xml:space="preserve">pargo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cubera amarilla</t>
+  </si>
+  <si>
     <t xml:space="preserve">cubera roja</t>
   </si>
   <si>
-    <t xml:space="preserve">pargo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cubera amarilla</t>
+    <t xml:space="preserve">cola amarilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motinsnapper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biajaiba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yellow-tail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motin snapper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef snapper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red-fish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pargo amarillo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">queensnapper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">butterfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dogteeth sn</t>
   </si>
   <si>
     <t xml:space="preserve">red snaper</t>
   </si>
   <si>
+    <t xml:space="preserve">curvina</t>
+  </si>
+  <si>
     <t xml:space="preserve">mutton snapper</t>
   </si>
   <si>
+    <t xml:space="preserve">queen snapper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">silk snapper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red fish</t>
+  </si>
+  <si>
     <t xml:space="preserve">red snaperj</t>
   </si>
   <si>
-    <t xml:space="preserve">yellow-tail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">red-fish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cola amarilla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pargo amarillo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">motin snapper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biajaiba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">queensnapper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">butterfish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">queen snapper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">motinsnapper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dogteeth sn</t>
+    <t xml:space="preserve">yellowtail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schoolmaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">long tail</t>
   </si>
   <si>
     <t xml:space="preserve">dogteethsnapper</t>
   </si>
   <si>
+    <t xml:space="preserve">snapper</t>
+  </si>
+  <si>
     <t xml:space="preserve">lane snapper</t>
   </si>
   <si>
-    <t xml:space="preserve">reef snapper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">curvina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schoolmaster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">red fish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">silk snapper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yellowtail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">long tail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">snapper</t>
-  </si>
-  <si>
     <t xml:space="preserve">Moronidae</t>
   </si>
   <si>
@@ -592,31 +592,31 @@
     <t xml:space="preserve">mero</t>
   </si>
   <si>
+    <t xml:space="preserve">jimmy hind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rockfish / yellowmouth grouper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rockfish / nassau grouper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rockfish / yellowfin grouper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rockfish / tiger grouper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yellowfin grouper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gruper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pez mantequilla</t>
+  </si>
+  <si>
     <t xml:space="preserve">jimmy hint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gruper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pez mantequilla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jimmy hind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rockfish / yellowmouth grouper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rockfish / nassau grouper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rockfish / yellowfin grouper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rockfish / tiger grouper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yellowfin grouper</t>
   </si>
   <si>
     <t xml:space="preserve">Serranidae</t>
@@ -2998,9 +2998,7 @@
       <c r="D92" t="s">
         <v>116</v>
       </c>
-      <c r="E92" t="s">
-        <v>141</v>
-      </c>
+      <c r="E92"/>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -3016,7 +3014,7 @@
         <v>116</v>
       </c>
       <c r="E93" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94">
@@ -3033,7 +3031,7 @@
         <v>116</v>
       </c>
       <c r="E94" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="95">
@@ -3050,7 +3048,7 @@
         <v>116</v>
       </c>
       <c r="E95" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="96">
@@ -3067,7 +3065,7 @@
         <v>116</v>
       </c>
       <c r="E96" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="97">
@@ -3083,7 +3081,9 @@
       <c r="D97" t="s">
         <v>116</v>
       </c>
-      <c r="E97"/>
+      <c r="E97" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -3250,7 +3250,7 @@
         <v>156</v>
       </c>
       <c r="E107" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="108">
@@ -3639,7 +3639,7 @@
         <v>187</v>
       </c>
       <c r="E130" t="s">
-        <v>192</v>
+        <v>138</v>
       </c>
     </row>
     <row r="131">
@@ -3656,7 +3656,7 @@
         <v>187</v>
       </c>
       <c r="E131" t="s">
-        <v>139</v>
+        <v>192</v>
       </c>
     </row>
     <row r="132">
@@ -3996,7 +3996,7 @@
         <v>206</v>
       </c>
       <c r="E151" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="152">
@@ -4013,7 +4013,7 @@
         <v>206</v>
       </c>
       <c r="E152" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="153">
@@ -5303,7 +5303,7 @@
         <v>260</v>
       </c>
       <c r="F57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58">
@@ -5561,7 +5561,7 @@
         <v>262</v>
       </c>
       <c r="F70" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71">
@@ -5581,7 +5581,7 @@
         <v>262</v>
       </c>
       <c r="F71" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72">
@@ -5601,7 +5601,7 @@
         <v>262</v>
       </c>
       <c r="F72" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="73">
@@ -5621,7 +5621,7 @@
         <v>262</v>
       </c>
       <c r="F73" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="74">
@@ -5640,9 +5640,7 @@
       <c r="E74" t="s">
         <v>262</v>
       </c>
-      <c r="F74" t="s">
-        <v>135</v>
-      </c>
+      <c r="F74"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -5661,7 +5659,7 @@
         <v>262</v>
       </c>
       <c r="F75" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76">
@@ -5681,7 +5679,7 @@
         <v>262</v>
       </c>
       <c r="F76" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77">
@@ -5700,7 +5698,9 @@
       <c r="E77" t="s">
         <v>262</v>
       </c>
-      <c r="F77"/>
+      <c r="F77" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -5719,7 +5719,7 @@
         <v>262</v>
       </c>
       <c r="F78" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="79">
@@ -5739,7 +5739,7 @@
         <v>262</v>
       </c>
       <c r="F79" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80">
@@ -5819,7 +5819,7 @@
         <v>262</v>
       </c>
       <c r="F83" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84">
@@ -5859,7 +5859,7 @@
         <v>263</v>
       </c>
       <c r="F85" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="86">
@@ -5879,7 +5879,7 @@
         <v>263</v>
       </c>
       <c r="F86" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="87">
@@ -5917,7 +5917,7 @@
         <v>263</v>
       </c>
       <c r="F88" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="89">
@@ -5937,7 +5937,7 @@
         <v>263</v>
       </c>
       <c r="F89" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="90">
@@ -6015,7 +6015,7 @@
         <v>267</v>
       </c>
       <c r="F93" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94">
@@ -6055,7 +6055,7 @@
         <v>269</v>
       </c>
       <c r="F95" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="96">
@@ -6453,7 +6453,7 @@
         <v>281</v>
       </c>
       <c r="F115" t="s">
-        <v>192</v>
+        <v>138</v>
       </c>
     </row>
     <row r="116">
@@ -6473,7 +6473,7 @@
         <v>281</v>
       </c>
       <c r="F116" t="s">
-        <v>139</v>
+        <v>192</v>
       </c>
     </row>
     <row r="117">
@@ -6513,7 +6513,7 @@
         <v>281</v>
       </c>
       <c r="F118" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="119">
@@ -6533,7 +6533,7 @@
         <v>281</v>
       </c>
       <c r="F119" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="120">
@@ -6553,7 +6553,7 @@
         <v>282</v>
       </c>
       <c r="F120" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="121">
@@ -6573,7 +6573,7 @@
         <v>282</v>
       </c>
       <c r="F121" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="122">
@@ -6593,7 +6593,7 @@
         <v>282</v>
       </c>
       <c r="F122" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="123">
@@ -6613,7 +6613,7 @@
         <v>282</v>
       </c>
       <c r="F123" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="124">
@@ -6673,7 +6673,7 @@
         <v>284</v>
       </c>
       <c r="F126" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="127">
@@ -6793,7 +6793,7 @@
         <v>286</v>
       </c>
       <c r="F132" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="133">
@@ -7315,7 +7315,7 @@
         <v>305</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17">
@@ -7476,7 +7476,7 @@
         <v>309</v>
       </c>
       <c r="G23" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24">
@@ -7499,7 +7499,7 @@
         <v>309</v>
       </c>
       <c r="G24" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25">
@@ -8051,7 +8051,7 @@
         <v>325</v>
       </c>
       <c r="G48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49">
@@ -8074,7 +8074,7 @@
         <v>326</v>
       </c>
       <c r="G49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50">
@@ -8164,7 +8164,7 @@
         <v>328</v>
       </c>
       <c r="G53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54">
@@ -8186,9 +8186,7 @@
       <c r="F54" t="s">
         <v>328</v>
       </c>
-      <c r="G54" t="s">
-        <v>130</v>
-      </c>
+      <c r="G54"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -8209,7 +8207,9 @@
       <c r="F55" t="s">
         <v>328</v>
       </c>
-      <c r="G55"/>
+      <c r="G55" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -8231,7 +8231,7 @@
         <v>329</v>
       </c>
       <c r="G56" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57">
@@ -8254,7 +8254,7 @@
         <v>329</v>
       </c>
       <c r="G57" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58">
@@ -8277,7 +8277,7 @@
         <v>330</v>
       </c>
       <c r="G58" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59">
@@ -8321,7 +8321,7 @@
         <v>331</v>
       </c>
       <c r="G60" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61">
@@ -8413,7 +8413,7 @@
         <v>334</v>
       </c>
       <c r="G64" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65">
@@ -8459,7 +8459,7 @@
         <v>335</v>
       </c>
       <c r="G66" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67">
@@ -8482,7 +8482,7 @@
         <v>335</v>
       </c>
       <c r="G67" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68">
@@ -8526,7 +8526,7 @@
         <v>335</v>
       </c>
       <c r="G69" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70">
@@ -8549,7 +8549,7 @@
         <v>335</v>
       </c>
       <c r="G70" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="71">
@@ -8616,7 +8616,7 @@
         <v>338</v>
       </c>
       <c r="G73" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74">
@@ -8662,7 +8662,7 @@
         <v>340</v>
       </c>
       <c r="G75" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76">
@@ -9005,7 +9005,7 @@
         <v>351</v>
       </c>
       <c r="G90" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91">
@@ -9028,7 +9028,7 @@
         <v>352</v>
       </c>
       <c r="G91" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="92">
@@ -9051,7 +9051,7 @@
         <v>353</v>
       </c>
       <c r="G92" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="93">
@@ -9074,7 +9074,7 @@
         <v>354</v>
       </c>
       <c r="G93" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="94">
@@ -9097,7 +9097,7 @@
         <v>355</v>
       </c>
       <c r="G94" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="95">
@@ -9120,7 +9120,7 @@
         <v>355</v>
       </c>
       <c r="G95" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="96">
@@ -9189,7 +9189,7 @@
         <v>357</v>
       </c>
       <c r="G98" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="99">
@@ -9304,7 +9304,7 @@
         <v>319</v>
       </c>
       <c r="G103" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="104">

</xml_diff>